<commit_message>
user add kora baki
</commit_message>
<xml_diff>
--- a/afar_project/csv_path/frc_asset_schedule.xlsx
+++ b/afar_project/csv_path/frc_asset_schedule.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,7 +439,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Accumulated Purchases( Post MAB)</t>
+          <t>Opening Balance</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -449,55 +449,65 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>Cost of asset sold</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Current Balance</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
         <is>
           <t>Rate ( Pre MAB Assets)</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Rate ( Post MAB Assets)</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Accumulated Depreciation</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Depreciation ( Pre MAB)</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Depreciation (Post MAB)</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>Depreciation ( New Purchases)</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>Depreciation Charges</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>Total Accumulated Depreciation</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>WDV</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
@@ -516,44 +526,50 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>65</v>
+        <v>2214149.3</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="inlineStr">
+        <v>2214149.3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2214149.3</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>20.00%</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
       <c r="K2" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>13</v>
+        <v>442829.86</v>
       </c>
       <c r="N2" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>52</v>
-      </c>
-      <c r="P2" t="inlineStr"/>
+        <v>442829.86</v>
+      </c>
+      <c r="P2" t="n">
+        <v>442829.86</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1771319.44</v>
+      </c>
+      <c r="R2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -568,44 +584,50 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>635</v>
+        <v>3623967</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>635</v>
+        <v>1686182</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="inlineStr">
+        <v>3623967</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1937785</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>14.29%</t>
         </is>
       </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
       <c r="K3" t="n">
-        <v>90.70999999999999</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>90.70999999999999</v>
+        <v>517709.57</v>
       </c>
       <c r="N3" t="n">
-        <v>90.70999999999999</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>544.29</v>
-      </c>
-      <c r="P3" t="inlineStr"/>
+        <v>517709.57</v>
+      </c>
+      <c r="P3" t="n">
+        <v>517709.57</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>3106257.43</v>
+      </c>
+      <c r="R3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -620,44 +642,50 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>169</v>
+        <v>3111004.93</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>169</v>
+        <v>1367021.79</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="inlineStr">
+        <v>3111004.93</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1743983.14</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>10.00%</t>
         </is>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
       <c r="K4" t="n">
-        <v>16.9</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>16.9</v>
+        <v>311100.49</v>
       </c>
       <c r="N4" t="n">
-        <v>16.9</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>152.1</v>
-      </c>
-      <c r="P4" t="inlineStr"/>
+        <v>311100.49</v>
+      </c>
+      <c r="P4" t="n">
+        <v>311100.49</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2799904.44</v>
+      </c>
+      <c r="R4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -672,44 +700,50 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>334523</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="inlineStr">
+        <v>334523</v>
+      </c>
+      <c r="H5" t="n">
+        <v>334523</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>14.29%</t>
         </is>
       </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
       <c r="K5" t="n">
-        <v>1.43</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>1.43</v>
+        <v>47789</v>
       </c>
       <c r="N5" t="n">
-        <v>1.43</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>8.57</v>
-      </c>
-      <c r="P5" t="inlineStr"/>
+        <v>47789</v>
+      </c>
+      <c r="P5" t="n">
+        <v>47789</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>286734</v>
+      </c>
+      <c r="R5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -724,44 +758,50 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>21671646</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="inlineStr">
+        <v>21671646</v>
+      </c>
+      <c r="H6" t="n">
+        <v>21671646</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>10.00%</t>
         </is>
       </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
       <c r="K6" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.7</v>
+        <v>2167164.6</v>
       </c>
       <c r="N6" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="P6" t="inlineStr"/>
+        <v>2167164.6</v>
+      </c>
+      <c r="P6" t="n">
+        <v>2167164.6</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>19504481.4</v>
+      </c>
+      <c r="R6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -776,44 +816,50 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>549298.2</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="inlineStr">
+        <v>549298.2</v>
+      </c>
+      <c r="H7" t="n">
+        <v>549298.2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="inlineStr">
         <is>
           <t>5.00%</t>
         </is>
       </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
       <c r="K7" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.5</v>
+        <v>27464.91</v>
       </c>
       <c r="N7" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="P7" t="inlineStr"/>
+        <v>27464.91</v>
+      </c>
+      <c r="P7" t="n">
+        <v>27464.91</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>521833.29</v>
+      </c>
+      <c r="R7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -828,44 +874,50 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>364</v>
+        <v>718355</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>364</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="inlineStr">
+        <v>718355</v>
+      </c>
+      <c r="H8" t="n">
+        <v>718355</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="inlineStr">
         <is>
           <t>6.67%</t>
         </is>
       </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
       <c r="K8" t="n">
-        <v>24.27</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>24.27</v>
+        <v>47890.33</v>
       </c>
       <c r="N8" t="n">
-        <v>24.27</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>339.73</v>
-      </c>
-      <c r="P8" t="inlineStr"/>
+        <v>47890.33</v>
+      </c>
+      <c r="P8" t="n">
+        <v>47890.33</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>670464.67</v>
+      </c>
+      <c r="R8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -880,44 +932,50 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>11</v>
+        <v>66900</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="inlineStr">
+        <v>66900</v>
+      </c>
+      <c r="H9" t="n">
+        <v>66900</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="inlineStr">
         <is>
           <t>6.67%</t>
         </is>
       </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
       <c r="K9" t="n">
-        <v>0.73</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.73</v>
+        <v>4460</v>
       </c>
       <c r="N9" t="n">
-        <v>0.73</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>10.27</v>
-      </c>
-      <c r="P9" t="inlineStr"/>
+        <v>4460</v>
+      </c>
+      <c r="P9" t="n">
+        <v>4460</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>62440</v>
+      </c>
+      <c r="R9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -932,44 +990,50 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>83</v>
+        <v>607855</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="inlineStr">
+        <v>607855</v>
+      </c>
+      <c r="H10" t="n">
+        <v>607855</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="inlineStr">
         <is>
           <t>5.00%</t>
         </is>
       </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
       <c r="K10" t="n">
-        <v>4.15</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>4.15</v>
+        <v>30392.75</v>
       </c>
       <c r="N10" t="n">
-        <v>4.15</v>
+        <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>78.84999999999999</v>
-      </c>
-      <c r="P10" t="inlineStr"/>
+        <v>30392.75</v>
+      </c>
+      <c r="P10" t="n">
+        <v>30392.75</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>577462.25</v>
+      </c>
+      <c r="R10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -984,44 +1048,50 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>750</v>
+        <v>1402841.25</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="inlineStr">
+        <v>1402841.25</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1402841.25</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>6.67%</t>
         </is>
       </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
       <c r="K11" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>50</v>
+        <v>93522.75</v>
       </c>
       <c r="N11" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>700</v>
-      </c>
-      <c r="P11" t="inlineStr"/>
+        <v>93522.75</v>
+      </c>
+      <c r="P11" t="n">
+        <v>93522.75</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>1309318.5</v>
+      </c>
+      <c r="R11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1036,44 +1106,50 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>5</v>
+        <v>375968.75</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="inlineStr">
+        <v>375968.75</v>
+      </c>
+      <c r="H12" t="n">
+        <v>375968.75</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="inlineStr">
         <is>
           <t>10.00%</t>
         </is>
       </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
       <c r="K12" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.5</v>
+        <v>37596.88</v>
       </c>
       <c r="N12" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="P12" t="inlineStr"/>
+        <v>37596.88</v>
+      </c>
+      <c r="P12" t="n">
+        <v>37596.88</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>338371.87</v>
+      </c>
+      <c r="R12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1088,44 +1164,50 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>66</v>
+        <v>4733279.250000001</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="inlineStr">
+        <v>4733279.25</v>
+      </c>
+      <c r="H13" t="n">
+        <v>4733279.25</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="inlineStr">
         <is>
           <t>5.00%</t>
         </is>
       </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
       <c r="K13" t="n">
-        <v>3.3</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>3.3</v>
+        <v>236663.96</v>
       </c>
       <c r="N13" t="n">
-        <v>3.3</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>62.7</v>
-      </c>
-      <c r="P13" t="inlineStr"/>
+        <v>236663.96</v>
+      </c>
+      <c r="P13" t="n">
+        <v>236663.96</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>4496615.29</v>
+      </c>
+      <c r="R13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1140,44 +1222,50 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>281</v>
+        <v>4771077.5</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>281</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="inlineStr">
+        <v>4771077.5</v>
+      </c>
+      <c r="H14" t="n">
+        <v>4771077.5</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="inlineStr">
         <is>
           <t>6.67%</t>
         </is>
       </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
       <c r="K14" t="n">
-        <v>18.73</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
         <v>0</v>
       </c>
       <c r="M14" t="n">
-        <v>18.73</v>
+        <v>318071.83</v>
       </c>
       <c r="N14" t="n">
-        <v>18.73</v>
+        <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>262.27</v>
-      </c>
-      <c r="P14" t="inlineStr"/>
+        <v>318071.83</v>
+      </c>
+      <c r="P14" t="n">
+        <v>318071.83</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>4453005.67</v>
+      </c>
+      <c r="R14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>